<commit_message>
Fixing code in Devil in HMl script for data raw and commodity in the long run
</commit_message>
<xml_diff>
--- a/sandbox/AQR_commodity.xlsx
+++ b/sandbox/AQR_commodity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\aqrcapital.com\shares\fs006\commodities\_data\long term com data library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED37706-372E-45C7-B6F9-9502696CAA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB78C0BF-1D03-493A-B4A4-0DA24A1909B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commodities for the Long Run" sheetId="55" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Data Sources" sheetId="38" r:id="rId3"/>
     <sheet name="Disclosures" sheetId="39" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="1"/>
+  <calcPr calcId="1" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3832" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3836" uniqueCount="305">
   <si>
     <t>Please see disclosures on the Disclosures tab.</t>
   </si>
@@ -2611,7 +2611,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1777"/>
+  <dimension ref="A1:L1779"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
@@ -69780,38 +69780,114 @@
         <v>28</v>
       </c>
     </row>
-    <row r="1777" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1777" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1777" s="26">
         <v>45380</v>
       </c>
       <c r="B1777" s="17">
-        <v>3.7213131757143851E-2</v>
+        <v>3.7213131757764931E-2</v>
       </c>
       <c r="C1777" s="17">
-        <v>4.0239041287861668E-2</v>
+        <v>4.0239041289942178E-2</v>
       </c>
       <c r="D1777" s="17">
-        <v>-2.278984815187905E-3</v>
+        <v>-2.2789848162716457E-3</v>
       </c>
       <c r="E1777" s="17">
-        <v>4.5046143378285601E-2</v>
+        <v>4.5046143380375749E-2</v>
       </c>
       <c r="F1777" s="17">
-        <v>-6.8683963049528101E-3</v>
+        <v>-6.8683963060315704E-3</v>
       </c>
       <c r="G1777" s="17">
-        <v>7.8493101347142449E-2</v>
+        <v>7.849310134536433E-2</v>
       </c>
       <c r="H1777" s="17">
-        <v>3.8100974023099775E-2</v>
+        <v>3.8100974024442964E-2</v>
       </c>
       <c r="I1777" s="17">
-        <v>3.763322165327479E-2</v>
+        <v>3.7633221650410248E-2</v>
       </c>
       <c r="J1777" s="17">
         <v>-3.688427177311669E-3</v>
       </c>
       <c r="K1777" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1777" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1778" s="26">
+        <v>45412</v>
+      </c>
+      <c r="B1778" s="17">
+        <v>2.0140336460879257E-2</v>
+      </c>
+      <c r="C1778" s="17">
+        <v>2.238739933360983E-2</v>
+      </c>
+      <c r="D1778" s="17">
+        <v>-1.5197525655093723E-3</v>
+      </c>
+      <c r="E1778" s="17">
+        <v>2.7138072192766999E-2</v>
+      </c>
+      <c r="F1778" s="17">
+        <v>-6.1378785412753182E-3</v>
+      </c>
+      <c r="G1778" s="17">
+        <v>-1.6569056128615454E-2</v>
+      </c>
+      <c r="H1778" s="17">
+        <v>-5.7564179001387536E-2</v>
+      </c>
+      <c r="I1778" s="17">
+        <v>4.0100642832792133E-2</v>
+      </c>
+      <c r="J1778" s="17">
+        <v>-4.0118166984945006E-3</v>
+      </c>
+      <c r="K1778" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1778" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1779" s="26">
+        <v>45443</v>
+      </c>
+      <c r="B1779" s="17">
+        <v>1.1618616057455872E-2</v>
+      </c>
+      <c r="C1779" s="17">
+        <v>1.4300133571822781E-2</v>
+      </c>
+      <c r="D1779" s="17">
+        <v>-1.5733328237808083E-3</v>
+      </c>
+      <c r="E1779" s="17">
+        <v>1.9033465870773862E-2</v>
+      </c>
+      <c r="F1779" s="17">
+        <v>-6.2109481231379937E-3</v>
+      </c>
+      <c r="G1779" s="17">
+        <v>-8.5209298817572277E-2</v>
+      </c>
+      <c r="H1779" s="17">
+        <v>-0.10914502120935489</v>
+      </c>
+      <c r="I1779" s="17">
+        <v>2.1314914123296776E-2</v>
+      </c>
+      <c r="J1779" s="17">
+        <v>-5.8434615149332717E-3</v>
+      </c>
+      <c r="K1779" s="20" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing errors and warnings in build
</commit_message>
<xml_diff>
--- a/sandbox/AQR_commodity.xlsx
+++ b/sandbox/AQR_commodity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\aqrcapital.com\shares\fs006\commodities\_data\long term com data library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB78C0BF-1D03-493A-B4A4-0DA24A1909B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBF67CF-8060-4222-9DDE-929558A40DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39570" yWindow="1170" windowWidth="28800" windowHeight="17175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commodities for the Long Run" sheetId="55" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Data Sources" sheetId="38" r:id="rId3"/>
     <sheet name="Disclosures" sheetId="39" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="1" concurrentCalc="0"/>
+  <calcPr calcId="1" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3836" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3840" uniqueCount="305">
   <si>
     <t>Please see disclosures on the Disclosures tab.</t>
   </si>
@@ -2291,9 +2291,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2331,9 +2331,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2366,26 +2366,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2418,26 +2401,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2611,7 +2577,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1779"/>
+  <dimension ref="A1:L1781"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
@@ -69861,34 +69827,110 @@
         <v>45443</v>
       </c>
       <c r="B1779" s="17">
-        <v>1.1618616057455872E-2</v>
+        <v>1.1618616055030921E-2</v>
       </c>
       <c r="C1779" s="17">
-        <v>1.4300133571822781E-2</v>
+        <v>1.4300133569838993E-2</v>
       </c>
       <c r="D1779" s="17">
-        <v>-1.5733328237808083E-3</v>
+        <v>-1.5733328242321359E-3</v>
       </c>
       <c r="E1779" s="17">
-        <v>1.9033465870773862E-2</v>
+        <v>1.9033465868780821E-2</v>
       </c>
       <c r="F1779" s="17">
-        <v>-6.2109481231379937E-3</v>
+        <v>-6.2109481235872246E-3</v>
       </c>
       <c r="G1779" s="17">
-        <v>-8.5209298817572277E-2</v>
+        <v>-8.5209298812436302E-2</v>
       </c>
       <c r="H1779" s="17">
-        <v>-0.10914502120935489</v>
+        <v>-0.10914502120550508</v>
       </c>
       <c r="I1779" s="17">
-        <v>2.1314914123296776E-2</v>
+        <v>2.1314914124719083E-2</v>
       </c>
       <c r="J1779" s="17">
         <v>-5.8434615149332717E-3</v>
       </c>
       <c r="K1779" s="20" t="s">
         <v>26</v>
+      </c>
+      <c r="L1779" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1780" s="26">
+        <v>45471</v>
+      </c>
+      <c r="B1780" s="17">
+        <v>-2.8142210149479225E-2</v>
+      </c>
+      <c r="C1780" s="17">
+        <v>-3.2659094244706158E-2</v>
+      </c>
+      <c r="D1780" s="17">
+        <v>4.9283781093456313E-3</v>
+      </c>
+      <c r="E1780" s="17">
+        <v>-2.8139007783793076E-2</v>
+      </c>
+      <c r="F1780" s="17">
+        <v>2.5449656408360236E-4</v>
+      </c>
+      <c r="G1780" s="17">
+        <v>5.3039282407797428E-2</v>
+      </c>
+      <c r="H1780" s="17">
+        <v>2.5579396222780187E-2</v>
+      </c>
+      <c r="I1780" s="17">
+        <v>3.037035530670594E-2</v>
+      </c>
+      <c r="J1780" s="17">
+        <v>-2.5983486603095695E-3</v>
+      </c>
+      <c r="K1780" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1780" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1781" s="26">
+        <v>45504</v>
+      </c>
+      <c r="B1781" s="17">
+        <v>-4.4713525932405761E-2</v>
+      </c>
+      <c r="C1781" s="17">
+        <v>-5.4639449670059022E-2</v>
+      </c>
+      <c r="D1781" s="17">
+        <v>1.1351728611579362E-2</v>
+      </c>
+      <c r="E1781" s="17">
+        <v>-5.021939343947792E-2</v>
+      </c>
+      <c r="F1781" s="17">
+        <v>6.6451348166746702E-3</v>
+      </c>
+      <c r="G1781" s="17">
+        <v>1.8651462692623466E-2</v>
+      </c>
+      <c r="H1781" s="17">
+        <v>-8.9443004275711856E-3</v>
+      </c>
+      <c r="I1781" s="17">
+        <v>3.1297570092104668E-2</v>
+      </c>
+      <c r="J1781" s="17">
+        <v>1.7977005364474123E-3</v>
+      </c>
+      <c r="K1781" s="20" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>